<commit_message>
thay doi cau truc thu muc
</commit_message>
<xml_diff>
--- a/copy_test_upload.xlsx
+++ b/copy_test_upload.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <r>
       <t>description</t>
     </r>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <r>
@@ -318,6 +315,85 @@
         <u val="single"/>
       </rPr>
       <t>dòng 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">in đậm.    </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">, test.     này là </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">in      nghiệm.   , </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow (Body)"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="single"/>
+      </rPr>
+      <t>underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>chỗ này là xuống 2 và</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow (Body)"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <color theme="1"/>
+        <sz val="12"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve"> dòng
+dòng 1
+dòng 2
+dòng 3</t>
     </r>
   </si>
 </sst>
@@ -632,96 +708,70 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>1</v>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>